<commit_message>
Added delays in 'GetPoolInventory'
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmahe\Documents\UiPath\PoolCleansingPOC\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314CA542-D528-46BE-AB10-A033DDF6774A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B8335E-4E38-4AD6-9568-9D19A6093867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,30 @@
   </si>
   <si>
     <t>Shared/PoolCleansing</t>
+  </si>
+  <si>
+    <t>YearFrom</t>
+  </si>
+  <si>
+    <t>MonthFrom</t>
+  </si>
+  <si>
+    <t>DateFrom</t>
+  </si>
+  <si>
+    <t>YearTo</t>
+  </si>
+  <si>
+    <t>MonthTo</t>
+  </si>
+  <si>
+    <t>DateTo</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>January</t>
   </si>
 </sst>
 </file>
@@ -211,14 +235,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +559,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -581,18 +604,18 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" s="4" customFormat="1" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="4" customFormat="1" ht="14.5">
+    <row r="3" spans="1:26" ht="14.5">
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
@@ -603,11 +626,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="4" customFormat="1" ht="14.5">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:26" ht="14.5">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -615,13 +638,55 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>25</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>